<commit_message>
+ added the empty_return_type attribute so that this package will emulate ParseExcel 	You can still choose to return undef by setting this attribute to 'undef_string' ! added another fix in the cleanup since it forced a fail when fails weren't needed
</commit_message>
<xml_diff>
--- a/Presentation/Date Examples.xlsx
+++ b/Presentation/Date Examples.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="19560" windowHeight="6465"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="9105" windowHeight="6195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\ mmmm\ d\,\ h:mm\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="yyyy\ mmmm\ d\,\ h:mm\ AM/PM"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -204,16 +204,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
@@ -223,15 +231,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,7 +530,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -539,6 +540,7 @@
     <col min="3" max="3" width="26.8984375" customWidth="1"/>
     <col min="4" max="5" width="3.296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -550,7 +552,7 @@
         <f>A1</f>
         <v>62.5</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F1" s="1"/>
@@ -563,7 +565,7 @@
         <f t="shared" ref="B2:B13" si="0">A2</f>
         <v>61.5</v>
       </c>
-      <c r="D2" s="10"/>
+      <c r="D2" s="12"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:9">
@@ -577,7 +579,7 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="10"/>
+      <c r="D3" s="12"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:9">
@@ -588,7 +590,7 @@
         <f t="shared" si="0"/>
         <v>59.5</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="12"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:9">
@@ -599,7 +601,7 @@
         <f t="shared" si="0"/>
         <v>58.5</v>
       </c>
-      <c r="D5" s="10"/>
+      <c r="D5" s="12"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:9">
@@ -610,8 +612,10 @@
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="D6" s="12"/>
       <c r="F6" s="1"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7">
@@ -621,8 +625,10 @@
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="12"/>
       <c r="F7" s="1"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8">
@@ -632,12 +638,13 @@
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="D8" s="10"/>
+      <c r="D8" s="12"/>
       <c r="F8" s="1"/>
       <c r="G8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="H8" s="2"/>
+      <c r="I8" s="14" t="s">
         <v>5</v>
       </c>
     </row>
@@ -645,38 +652,40 @@
       <c r="A9">
         <v>0.5</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="10"/>
+      <c r="D9" s="12"/>
       <c r="F9" s="1">
         <v>2</v>
       </c>
-      <c r="I9" s="6"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10">
         <v>-0.5</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="7">
         <f t="shared" si="0"/>
         <v>-0.5</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="12" t="s">
+      <c r="D10" s="12"/>
+      <c r="E10" s="8" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="H10" s="2"/>
+      <c r="I10" s="14" t="s">
         <v>6</v>
       </c>
     </row>
@@ -684,19 +693,21 @@
       <c r="A11">
         <v>-1.5</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="7">
         <f t="shared" si="0"/>
         <v>-1.5</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="13"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="9"/>
       <c r="F11" s="1"/>
       <c r="G11" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
@@ -709,9 +720,11 @@
       <c r="C12" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="13"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="9"/>
       <c r="F12" s="1"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" ht="19.5" thickBot="1">
       <c r="A13" t="s">
@@ -724,9 +737,11 @@
       <c r="C13" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="14"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="10"/>
       <c r="F13" s="1"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9">
       <c r="F14" s="1"/>

</xml_diff>